<commit_message>
updating data, cleaning up code
</commit_message>
<xml_diff>
--- a/_input/acs_dict.xlsx
+++ b/_input/acs_dict.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennah/code/cb3-census-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennah/code/cb3-census-data/_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A70DA7-F66F-BC4C-A1A7-7934235C4722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76CBF67-69A1-2D45-B265-0EB9C09C2287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{139C5A94-ED69-B840-976C-53C9B26A8F22}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="342">
   <si>
     <t>colname</t>
   </si>
@@ -1022,6 +1022,51 @@
   </si>
   <si>
     <t>not_in_2013</t>
+  </si>
+  <si>
+    <t>B08124_001E</t>
+  </si>
+  <si>
+    <t>total_occupation</t>
+  </si>
+  <si>
+    <t>B08124_002E</t>
+  </si>
+  <si>
+    <t>B08124_003E</t>
+  </si>
+  <si>
+    <t>service_occupation</t>
+  </si>
+  <si>
+    <t>management_business_occupation</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>B08124_004E</t>
+  </si>
+  <si>
+    <t>sales_office_occupation</t>
+  </si>
+  <si>
+    <t>B08124_005E</t>
+  </si>
+  <si>
+    <t>natural_res_construction_occupation</t>
+  </si>
+  <si>
+    <t>B08124_006E</t>
+  </si>
+  <si>
+    <t>production_transp_occupation</t>
+  </si>
+  <si>
+    <t>B08124_007E</t>
+  </si>
+  <si>
+    <t>military_occupation</t>
   </si>
 </sst>
 </file>
@@ -1439,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F22D90-69CC-424A-BF06-761D0AA8E975}">
-  <dimension ref="A1:X157"/>
+  <dimension ref="A1:X163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129:XFD129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5795,13 +5840,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>288</v>
@@ -5809,10 +5854,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>249</v>
@@ -5823,33 +5868,33 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>288</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="C131" s="2"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="C132" s="2"/>
+        <v>262</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>262</v>
@@ -5860,10 +5905,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>262</v>
@@ -5874,24 +5919,24 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>263</v>
@@ -5902,10 +5947,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>263</v>
@@ -5916,10 +5961,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>263</v>
@@ -5930,10 +5975,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>263</v>
@@ -5944,24 +5989,24 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>267</v>
+        <v>292</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>263</v>
+        <v>292</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>292</v>
@@ -5972,10 +6017,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>292</v>
@@ -5986,10 +6031,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>292</v>
@@ -6000,24 +6045,24 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>292</v>
+        <v>309</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>309</v>
@@ -6028,10 +6073,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>309</v>
@@ -6042,10 +6087,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>309</v>
@@ -6056,10 +6101,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>309</v>
@@ -6070,10 +6115,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>309</v>
@@ -6084,10 +6129,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>309</v>
@@ -6098,10 +6143,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>309</v>
@@ -6112,10 +6157,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>309</v>
@@ -6126,10 +6171,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>309</v>
@@ -6140,10 +6185,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>309</v>
@@ -6154,32 +6199,116 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="C155" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D155" s="2" t="s">
-        <v>310</v>
+        <v>323</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>325</v>
+        <v>328</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D157" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>